<commit_message>
ttest Signed-off-by: eagleduk <33012310+eagleduk@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ISS_Simulator/HE_SimulatorDT_H2400_100_.xlsx
+++ b/ISS_Simulator/HE_SimulatorDT_H2400_100_.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjlee\git\Simulator\ISS_Simulator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B545FB-B8C1-45D9-AF4D-B1552BBBD90F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="330" windowWidth="22005" windowHeight="13950"/>
+    <workbookView xWindow="1515" yWindow="330" windowWidth="22005" windowHeight="13950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="80">
   <si>
     <t>RedisKey</t>
   </si>
@@ -253,14 +259,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Fuel Oil Temp. Inlet Engine</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Volume flow</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Fuel Oil Press. Inlet Engine</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -271,43 +269,7 @@
     <t>Charge Air Pressure After A/C</t>
   </si>
   <si>
-    <t>Exh. Gas Temp. T/C Inlet A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exh. Gas Temp. T/C Inlet B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exh Gas Temp. T/C Outlet</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>C.W. to Air Cooler</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exh. Gas Temp. Out. Cyl. No.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exh. Gas Temp. Out. Cyl. No.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exh. Gas Temp. Out. Cyl. No.3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exh. Gas Temp. Out. Cyl. No.4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exh. Gas Temp. Out. Cyl. No.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exh. Gas Temp. Out. Cyl. No.6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -322,44 +284,8 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>_GE1022</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>_GE1028</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>_GG001</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>_GE1048</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>_GE1049</t>
-  </si>
-  <si>
-    <t>_GE1050</t>
-  </si>
-  <si>
-    <t>_GE1051</t>
-  </si>
-  <si>
-    <t>_GE1052</t>
-  </si>
-  <si>
-    <t>_GE1053</t>
-  </si>
-  <si>
-    <t>_GE1058</t>
-  </si>
-  <si>
-    <t>_GE1095</t>
-  </si>
-  <si>
-    <t>_GE1057</t>
   </si>
   <si>
     <t>Longitudinal_water_speed</t>
@@ -376,7 +302,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
@@ -538,6 +464,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -585,7 +514,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -618,9 +547,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -653,6 +599,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -828,11 +791,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="A39" sqref="A39:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1346,7 +1309,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="2" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>58</v>
@@ -1365,7 +1328,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="3" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>59</v>
@@ -1441,7 +1404,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="7" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>66</v>
@@ -1460,7 +1423,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>67</v>
@@ -1481,7 +1444,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="2" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>68</v>
@@ -1502,7 +1465,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>69</v>
@@ -1510,14 +1473,20 @@
       <c r="C35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
+      <c r="D35" s="6">
+        <f>4.7*(1-0.01)</f>
+        <v>4.6530000000000005</v>
+      </c>
+      <c r="E35" s="6">
+        <f>4.7*(1+0.01)</f>
+        <v>4.7469999999999999</v>
+      </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="1" t="s">
-        <v>89</v>
+      <c r="A36" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>70</v>
@@ -1525,14 +1494,18 @@
       <c r="C36" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
+      <c r="D36" s="6">
+        <v>35</v>
+      </c>
+      <c r="E36" s="6">
+        <v>37</v>
+      </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="2" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>71</v>
@@ -1541,19 +1514,19 @@
         <v>6</v>
       </c>
       <c r="D37" s="6">
-        <f>4.7*(1-0.01)</f>
-        <v>4.6530000000000005</v>
+        <f>4.1*(1-0.01)</f>
+        <v>4.0589999999999993</v>
       </c>
       <c r="E37" s="6">
-        <f>4.7*(1+0.01)</f>
-        <v>4.7469999999999999</v>
+        <f>4.1*(1+0.01)</f>
+        <v>4.141</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="2" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>72</v>
@@ -1562,191 +1535,17 @@
         <v>6</v>
       </c>
       <c r="D38" s="6">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E38" s="6">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="6">
-        <f>4.1*(1-0.01)</f>
-        <v>4.0589999999999993</v>
-      </c>
-      <c r="E39" s="6">
-        <f>4.1*(1+0.01)</f>
-        <v>4.141</v>
-      </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" t="s">
-        <v>96</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" t="s">
-        <v>97</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" t="s">
-        <v>98</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="6">
-        <v>32</v>
-      </c>
-      <c r="E43" s="6">
-        <v>34</v>
-      </c>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>